<commit_message>
update test case order
</commit_message>
<xml_diff>
--- a/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
+++ b/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="110">
   <si>
     <t>VVSS, Info Romana, 2023-2024</t>
   </si>
@@ -267,24 +267,24 @@
     <t>F02_TC01</t>
   </si>
   <si>
+    <t>task(“title”, 1)</t>
+  </si>
+  <si>
+    <t>1, 3, 4, 5, 6, 7, 9, 11, 13, 15, 16</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>F02_TC02</t>
+  </si>
+  <si>
     <t>null</t>
   </si>
   <si>
     <t>1, 2</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>F01_TC02</t>
-  </si>
-  <si>
-    <t>task(“title”, 1)</t>
-  </si>
-  <si>
-    <t>1, 3, 4, 5, 6, 7, 9, 11, 13, 15, 16</t>
-  </si>
-  <si>
     <t>WBT Implemented TCs</t>
   </si>
   <si>
@@ -321,13 +321,10 @@
     <t>F02</t>
   </si>
   <si>
+    <t>“task”</t>
+  </si>
+  <si>
     <t>NULL</t>
-  </si>
-  <si>
-    <t>F02_TC02</t>
-  </si>
-  <si>
-    <t>“task”</t>
   </si>
   <si>
     <t>Statistics</t>
@@ -582,7 +579,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -638,11 +635,6 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="13"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -1445,26 +1437,26 @@
     <xf numFmtId="49" fontId="9" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="9" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="7" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
@@ -1529,7 +1521,7 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="9" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1586,10 +1578,10 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="13" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="14" fillId="13" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="13" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="14" fillId="13" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -4495,43 +4487,53 @@
         <v>73</v>
       </c>
       <c r="D10" t="b" s="80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s" s="81">
         <v>74</v>
       </c>
-      <c r="F10" t="s" s="82">
+      <c r="F10" s="82"/>
+      <c r="G10" t="s" s="83">
         <v>75</v>
       </c>
-      <c r="G10" s="83"/>
-      <c r="H10" s="83"/>
-      <c r="I10" s="83"/>
-      <c r="J10" s="83"/>
-      <c r="K10" s="83"/>
-      <c r="L10" s="83"/>
-      <c r="M10" s="83"/>
-      <c r="N10" s="83"/>
-      <c r="O10" s="83"/>
-      <c r="P10" s="83"/>
-      <c r="Q10" s="83"/>
-      <c r="R10" s="83"/>
-      <c r="S10" s="83"/>
-      <c r="T10" t="s" s="84">
+      <c r="H10" t="s" s="83">
         <v>75</v>
       </c>
-      <c r="U10" s="85"/>
-      <c r="V10" s="85"/>
-      <c r="W10" s="85"/>
-      <c r="X10" s="85"/>
-      <c r="Y10" s="85"/>
-      <c r="Z10" s="85"/>
-      <c r="AA10" s="86"/>
-      <c r="AB10" s="86"/>
-      <c r="AC10" s="86"/>
-      <c r="AD10" s="86"/>
-      <c r="AE10" s="86"/>
-      <c r="AF10" s="86"/>
-      <c r="AG10" s="86"/>
+      <c r="I10" s="82"/>
+      <c r="J10" t="s" s="83">
+        <v>75</v>
+      </c>
+      <c r="K10" s="82"/>
+      <c r="L10" s="82"/>
+      <c r="M10" t="s" s="83">
+        <v>75</v>
+      </c>
+      <c r="N10" s="82"/>
+      <c r="O10" t="s" s="83">
+        <v>75</v>
+      </c>
+      <c r="P10" s="82"/>
+      <c r="Q10" t="s" s="83">
+        <v>75</v>
+      </c>
+      <c r="R10" s="82"/>
+      <c r="S10" t="s" s="83">
+        <v>75</v>
+      </c>
+      <c r="T10" s="84"/>
+      <c r="U10" s="84"/>
+      <c r="V10" s="84"/>
+      <c r="W10" s="84"/>
+      <c r="X10" s="84"/>
+      <c r="Y10" s="84"/>
+      <c r="Z10" s="84"/>
+      <c r="AA10" s="85"/>
+      <c r="AB10" s="85"/>
+      <c r="AC10" s="85"/>
+      <c r="AD10" s="85"/>
+      <c r="AE10" s="85"/>
+      <c r="AF10" s="85"/>
+      <c r="AG10" s="85"/>
     </row>
     <row r="11" ht="15.6" customHeight="1">
       <c r="A11" s="4"/>
@@ -4542,53 +4544,43 @@
         <v>77</v>
       </c>
       <c r="D11" t="b" s="80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="s" s="81">
         <v>78</v>
       </c>
-      <c r="F11" s="83"/>
-      <c r="G11" t="s" s="82">
+      <c r="F11" t="s" s="83">
         <v>75</v>
       </c>
-      <c r="H11" t="s" s="82">
+      <c r="G11" s="82"/>
+      <c r="H11" s="82"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="82"/>
+      <c r="K11" s="82"/>
+      <c r="L11" s="82"/>
+      <c r="M11" s="82"/>
+      <c r="N11" s="82"/>
+      <c r="O11" s="82"/>
+      <c r="P11" s="82"/>
+      <c r="Q11" s="82"/>
+      <c r="R11" s="82"/>
+      <c r="S11" s="82"/>
+      <c r="T11" t="s" s="86">
         <v>75</v>
       </c>
-      <c r="I11" s="83"/>
-      <c r="J11" t="s" s="82">
-        <v>75</v>
-      </c>
-      <c r="K11" s="83"/>
-      <c r="L11" s="83"/>
-      <c r="M11" t="s" s="82">
-        <v>75</v>
-      </c>
-      <c r="N11" s="83"/>
-      <c r="O11" t="s" s="82">
-        <v>75</v>
-      </c>
-      <c r="P11" s="83"/>
-      <c r="Q11" t="s" s="82">
-        <v>75</v>
-      </c>
-      <c r="R11" s="83"/>
-      <c r="S11" t="s" s="82">
-        <v>75</v>
-      </c>
-      <c r="T11" s="85"/>
-      <c r="U11" s="85"/>
-      <c r="V11" s="85"/>
-      <c r="W11" s="85"/>
-      <c r="X11" s="85"/>
-      <c r="Y11" s="85"/>
-      <c r="Z11" s="85"/>
-      <c r="AA11" s="86"/>
-      <c r="AB11" s="86"/>
-      <c r="AC11" s="86"/>
-      <c r="AD11" s="86"/>
-      <c r="AE11" s="86"/>
-      <c r="AF11" s="86"/>
-      <c r="AG11" s="86"/>
+      <c r="U11" s="84"/>
+      <c r="V11" s="84"/>
+      <c r="W11" s="84"/>
+      <c r="X11" s="84"/>
+      <c r="Y11" s="84"/>
+      <c r="Z11" s="84"/>
+      <c r="AA11" s="85"/>
+      <c r="AB11" s="85"/>
+      <c r="AC11" s="85"/>
+      <c r="AD11" s="85"/>
+      <c r="AE11" s="85"/>
+      <c r="AF11" s="85"/>
+      <c r="AG11" s="85"/>
     </row>
     <row r="12" ht="15.6" customHeight="1">
       <c r="A12" s="4"/>
@@ -4598,34 +4590,34 @@
       <c r="C12" s="87"/>
       <c r="D12" s="88"/>
       <c r="E12" s="89"/>
-      <c r="F12" s="83"/>
-      <c r="G12" s="83"/>
-      <c r="H12" s="83"/>
-      <c r="I12" s="83"/>
-      <c r="J12" s="83"/>
-      <c r="K12" s="83"/>
-      <c r="L12" s="83"/>
-      <c r="M12" s="83"/>
-      <c r="N12" s="83"/>
-      <c r="O12" s="83"/>
-      <c r="P12" s="83"/>
-      <c r="Q12" s="83"/>
-      <c r="R12" s="83"/>
-      <c r="S12" s="83"/>
-      <c r="T12" s="85"/>
-      <c r="U12" s="85"/>
-      <c r="V12" s="85"/>
-      <c r="W12" s="85"/>
-      <c r="X12" s="85"/>
-      <c r="Y12" s="85"/>
-      <c r="Z12" s="85"/>
-      <c r="AA12" s="86"/>
-      <c r="AB12" s="86"/>
-      <c r="AC12" s="86"/>
-      <c r="AD12" s="86"/>
-      <c r="AE12" s="86"/>
-      <c r="AF12" s="86"/>
-      <c r="AG12" s="86"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="82"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="82"/>
+      <c r="K12" s="82"/>
+      <c r="L12" s="82"/>
+      <c r="M12" s="82"/>
+      <c r="N12" s="82"/>
+      <c r="O12" s="82"/>
+      <c r="P12" s="82"/>
+      <c r="Q12" s="82"/>
+      <c r="R12" s="82"/>
+      <c r="S12" s="82"/>
+      <c r="T12" s="84"/>
+      <c r="U12" s="84"/>
+      <c r="V12" s="84"/>
+      <c r="W12" s="84"/>
+      <c r="X12" s="84"/>
+      <c r="Y12" s="84"/>
+      <c r="Z12" s="84"/>
+      <c r="AA12" s="85"/>
+      <c r="AB12" s="85"/>
+      <c r="AC12" s="85"/>
+      <c r="AD12" s="85"/>
+      <c r="AE12" s="85"/>
+      <c r="AF12" s="85"/>
+      <c r="AG12" s="85"/>
     </row>
     <row r="13" ht="15.6" customHeight="1">
       <c r="A13" s="4"/>
@@ -4635,34 +4627,34 @@
       <c r="C13" s="90"/>
       <c r="D13" s="91"/>
       <c r="E13" s="89"/>
-      <c r="F13" s="83"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="83"/>
-      <c r="I13" s="83"/>
-      <c r="J13" s="83"/>
-      <c r="K13" s="83"/>
-      <c r="L13" s="83"/>
-      <c r="M13" s="83"/>
-      <c r="N13" s="83"/>
-      <c r="O13" s="83"/>
-      <c r="P13" s="83"/>
-      <c r="Q13" s="83"/>
-      <c r="R13" s="83"/>
-      <c r="S13" s="83"/>
-      <c r="T13" s="85"/>
-      <c r="U13" s="85"/>
-      <c r="V13" s="85"/>
-      <c r="W13" s="85"/>
-      <c r="X13" s="85"/>
-      <c r="Y13" s="85"/>
-      <c r="Z13" s="85"/>
-      <c r="AA13" s="86"/>
-      <c r="AB13" s="86"/>
-      <c r="AC13" s="86"/>
-      <c r="AD13" s="86"/>
-      <c r="AE13" s="86"/>
-      <c r="AF13" s="86"/>
-      <c r="AG13" s="86"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="82"/>
+      <c r="I13" s="82"/>
+      <c r="J13" s="82"/>
+      <c r="K13" s="82"/>
+      <c r="L13" s="82"/>
+      <c r="M13" s="82"/>
+      <c r="N13" s="82"/>
+      <c r="O13" s="82"/>
+      <c r="P13" s="82"/>
+      <c r="Q13" s="82"/>
+      <c r="R13" s="82"/>
+      <c r="S13" s="82"/>
+      <c r="T13" s="84"/>
+      <c r="U13" s="84"/>
+      <c r="V13" s="84"/>
+      <c r="W13" s="84"/>
+      <c r="X13" s="84"/>
+      <c r="Y13" s="84"/>
+      <c r="Z13" s="84"/>
+      <c r="AA13" s="85"/>
+      <c r="AB13" s="85"/>
+      <c r="AC13" s="85"/>
+      <c r="AD13" s="85"/>
+      <c r="AE13" s="85"/>
+      <c r="AF13" s="85"/>
+      <c r="AG13" s="85"/>
     </row>
     <row r="14" ht="15.6" customHeight="1">
       <c r="A14" s="4"/>
@@ -4672,34 +4664,34 @@
       <c r="C14" s="90"/>
       <c r="D14" s="91"/>
       <c r="E14" s="89"/>
-      <c r="F14" s="83"/>
-      <c r="G14" s="83"/>
-      <c r="H14" s="83"/>
-      <c r="I14" s="83"/>
-      <c r="J14" s="83"/>
-      <c r="K14" s="83"/>
-      <c r="L14" s="83"/>
-      <c r="M14" s="83"/>
-      <c r="N14" s="83"/>
-      <c r="O14" s="83"/>
-      <c r="P14" s="83"/>
-      <c r="Q14" s="83"/>
-      <c r="R14" s="83"/>
-      <c r="S14" s="83"/>
-      <c r="T14" s="85"/>
-      <c r="U14" s="85"/>
-      <c r="V14" s="85"/>
-      <c r="W14" s="85"/>
-      <c r="X14" s="85"/>
-      <c r="Y14" s="85"/>
-      <c r="Z14" s="85"/>
-      <c r="AA14" s="86"/>
-      <c r="AB14" s="86"/>
-      <c r="AC14" s="86"/>
-      <c r="AD14" s="86"/>
-      <c r="AE14" s="86"/>
-      <c r="AF14" s="86"/>
-      <c r="AG14" s="86"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="82"/>
+      <c r="K14" s="82"/>
+      <c r="L14" s="82"/>
+      <c r="M14" s="82"/>
+      <c r="N14" s="82"/>
+      <c r="O14" s="82"/>
+      <c r="P14" s="82"/>
+      <c r="Q14" s="82"/>
+      <c r="R14" s="82"/>
+      <c r="S14" s="82"/>
+      <c r="T14" s="84"/>
+      <c r="U14" s="84"/>
+      <c r="V14" s="84"/>
+      <c r="W14" s="84"/>
+      <c r="X14" s="84"/>
+      <c r="Y14" s="84"/>
+      <c r="Z14" s="84"/>
+      <c r="AA14" s="85"/>
+      <c r="AB14" s="85"/>
+      <c r="AC14" s="85"/>
+      <c r="AD14" s="85"/>
+      <c r="AE14" s="85"/>
+      <c r="AF14" s="85"/>
+      <c r="AG14" s="85"/>
     </row>
     <row r="15" ht="15.6" customHeight="1">
       <c r="A15" s="4"/>
@@ -4709,34 +4701,34 @@
       <c r="C15" s="90"/>
       <c r="D15" s="91"/>
       <c r="E15" s="89"/>
-      <c r="F15" s="83"/>
-      <c r="G15" s="83"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="83"/>
-      <c r="J15" s="83"/>
-      <c r="K15" s="83"/>
-      <c r="L15" s="83"/>
-      <c r="M15" s="83"/>
-      <c r="N15" s="83"/>
-      <c r="O15" s="83"/>
-      <c r="P15" s="83"/>
-      <c r="Q15" s="83"/>
-      <c r="R15" s="83"/>
-      <c r="S15" s="83"/>
-      <c r="T15" s="85"/>
-      <c r="U15" s="85"/>
-      <c r="V15" s="85"/>
-      <c r="W15" s="85"/>
-      <c r="X15" s="85"/>
-      <c r="Y15" s="85"/>
-      <c r="Z15" s="85"/>
-      <c r="AA15" s="86"/>
-      <c r="AB15" s="86"/>
-      <c r="AC15" s="86"/>
-      <c r="AD15" s="86"/>
-      <c r="AE15" s="86"/>
-      <c r="AF15" s="86"/>
-      <c r="AG15" s="86"/>
+      <c r="F15" s="82"/>
+      <c r="G15" s="82"/>
+      <c r="H15" s="82"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="82"/>
+      <c r="K15" s="82"/>
+      <c r="L15" s="82"/>
+      <c r="M15" s="82"/>
+      <c r="N15" s="82"/>
+      <c r="O15" s="82"/>
+      <c r="P15" s="82"/>
+      <c r="Q15" s="82"/>
+      <c r="R15" s="82"/>
+      <c r="S15" s="82"/>
+      <c r="T15" s="84"/>
+      <c r="U15" s="84"/>
+      <c r="V15" s="84"/>
+      <c r="W15" s="84"/>
+      <c r="X15" s="84"/>
+      <c r="Y15" s="84"/>
+      <c r="Z15" s="84"/>
+      <c r="AA15" s="85"/>
+      <c r="AB15" s="85"/>
+      <c r="AC15" s="85"/>
+      <c r="AD15" s="85"/>
+      <c r="AE15" s="85"/>
+      <c r="AF15" s="85"/>
+      <c r="AG15" s="85"/>
     </row>
     <row r="16" ht="15.6" customHeight="1">
       <c r="A16" s="2"/>
@@ -4960,13 +4952,13 @@
         <v>72</v>
       </c>
       <c r="E6" t="s" s="103">
+        <v>85</v>
+      </c>
+      <c r="F6" t="s" s="103">
         <v>91</v>
       </c>
-      <c r="F6" t="s" s="103">
-        <v>24</v>
-      </c>
-      <c r="G6" t="s" s="103">
-        <v>33</v>
+      <c r="G6" s="104">
+        <v>1</v>
       </c>
       <c r="H6" t="s" s="103">
         <v>24</v>
@@ -4976,7 +4968,7 @@
       </c>
       <c r="J6" s="100"/>
       <c r="K6" t="b" s="104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" t="s" s="103">
         <v>24</v>
@@ -4991,16 +4983,16 @@
       </c>
       <c r="C7" s="106"/>
       <c r="D7" t="s" s="103">
+        <v>76</v>
+      </c>
+      <c r="E7" t="s" s="103">
         <v>92</v>
       </c>
-      <c r="E7" t="s" s="103">
-        <v>85</v>
-      </c>
       <c r="F7" t="s" s="103">
-        <v>93</v>
-      </c>
-      <c r="G7" s="104">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="G7" t="s" s="103">
+        <v>33</v>
       </c>
       <c r="H7" t="s" s="103">
         <v>24</v>
@@ -5010,7 +5002,7 @@
       </c>
       <c r="J7" s="100"/>
       <c r="K7" t="b" s="104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" t="s" s="103">
         <v>24</v>
@@ -5024,32 +5016,16 @@
         <v>11</v>
       </c>
       <c r="C8" s="106"/>
-      <c r="D8" t="s" s="103">
-        <v>24</v>
-      </c>
-      <c r="E8" t="s" s="103">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s" s="103">
-        <v>24</v>
-      </c>
-      <c r="G8" t="s" s="103">
-        <v>33</v>
-      </c>
-      <c r="H8" t="s" s="103">
-        <v>24</v>
-      </c>
-      <c r="I8" t="s" s="98">
-        <v>24</v>
-      </c>
-      <c r="J8" s="100"/>
-      <c r="K8" t="s" s="103">
-        <v>24</v>
-      </c>
-      <c r="L8" t="s" s="103">
-        <v>24</v>
-      </c>
-      <c r="M8" s="8"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
@@ -5139,7 +5115,7 @@
     <row r="12" ht="14.7" customHeight="1">
       <c r="A12" s="2"/>
       <c r="B12" t="s" s="109">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
@@ -5157,67 +5133,67 @@
     <row r="13" ht="15" customHeight="1">
       <c r="A13" s="4"/>
       <c r="B13" t="s" s="111">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C13" s="112"/>
       <c r="D13" s="112"/>
       <c r="E13" s="112"/>
       <c r="F13" t="s" s="113">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G13" s="114"/>
       <c r="H13" t="s" s="111">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I13" s="112"/>
       <c r="J13" s="112"/>
       <c r="K13" s="112"/>
       <c r="L13" s="115"/>
       <c r="M13" t="s" s="116">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N13" s="117"/>
     </row>
     <row r="14" ht="14.7" customHeight="1">
       <c r="A14" s="4"/>
       <c r="B14" t="s" s="118">
+        <v>98</v>
+      </c>
+      <c r="C14" t="s" s="118">
         <v>99</v>
       </c>
-      <c r="C14" t="s" s="118">
+      <c r="D14" t="s" s="118">
         <v>100</v>
       </c>
-      <c r="D14" t="s" s="118">
+      <c r="E14" t="s" s="119">
         <v>101</v>
       </c>
-      <c r="E14" t="s" s="119">
+      <c r="F14" t="s" s="120">
         <v>102</v>
       </c>
-      <c r="F14" t="s" s="120">
+      <c r="G14" t="s" s="118">
         <v>103</v>
       </c>
-      <c r="G14" t="s" s="118">
+      <c r="H14" t="s" s="121">
         <v>104</v>
       </c>
-      <c r="H14" t="s" s="121">
+      <c r="I14" t="s" s="118">
+        <v>98</v>
+      </c>
+      <c r="J14" t="s" s="118">
+        <v>99</v>
+      </c>
+      <c r="K14" t="s" s="118">
         <v>105</v>
       </c>
-      <c r="I14" t="s" s="118">
-        <v>99</v>
-      </c>
-      <c r="J14" t="s" s="118">
-        <v>100</v>
-      </c>
-      <c r="K14" t="s" s="118">
+      <c r="L14" t="s" s="119">
         <v>106</v>
       </c>
-      <c r="L14" t="s" s="119">
+      <c r="M14" t="s" s="96">
         <v>107</v>
       </c>
-      <c r="M14" t="s" s="96">
+      <c r="N14" t="s" s="96">
         <v>108</v>
-      </c>
-      <c r="N14" t="s" s="96">
-        <v>109</v>
       </c>
     </row>
     <row r="15" ht="92.5" customHeight="1">
@@ -5251,10 +5227,10 @@
       <c r="E16" s="127"/>
       <c r="F16" s="128"/>
       <c r="G16" t="s" s="129">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H16" t="s" s="129">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I16" s="125">
         <f>SUM(J16:K16)</f>
@@ -5268,7 +5244,7 @@
       </c>
       <c r="L16" s="127"/>
       <c r="M16" t="s" s="130">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N16" s="126">
         <f>C16</f>
@@ -5289,10 +5265,7 @@
     <mergeCell ref="N14:N15"/>
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="I14:I15"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
     <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I8:J8"/>
     <mergeCell ref="J14:J15"/>
     <mergeCell ref="K14:K15"/>
     <mergeCell ref="D1:G1"/>
@@ -5308,6 +5281,9 @@
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="H13:L13"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>